<commit_message>
changed model paths file to better default
</commit_message>
<xml_diff>
--- a/model_paths/model_paths_and_files.xlsx
+++ b/model_paths/model_paths_and_files.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sindredenby/Documents/metrologisk/NORTRIP-python/model_paths/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{436354AD-1FF5-7C46-94CD-25BE706253C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{68C47AD9-3C6C-1E44-9E71-420FE8FA2C8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
   <si>
     <t>Model input data path</t>
   </si>
@@ -122,25 +122,28 @@
     <t>Road_dust_parameter_table_v9_Denby.xlsx</t>
   </si>
   <si>
-    <t>Road_dust_parameter_table_v11.xlsx</t>
-  </si>
-  <si>
     <t>TRV atgarder Sundsvall 250121_settings.xlsx</t>
   </si>
   <si>
-    <t>/Users/sindredenby/Documents/metrologisk/NORTRIP-python/model_parameters/</t>
-  </si>
-  <si>
-    <t>/Users/sindredenby/Documents/metrologisk/NORTRIP-python/input_data/</t>
-  </si>
-  <si>
-    <t>/Users/sindredenby/Documents/metrologisk/NORTRIP-python/output_data/</t>
-  </si>
-  <si>
-    <t>/Users/sindredenby/Documents/metrologisk/NORTRIP-python/output_figures/</t>
-  </si>
-  <si>
-    <t>hello.xlsx</t>
+    <t>model_parameters/</t>
+  </si>
+  <si>
+    <t>input_data/</t>
+  </si>
+  <si>
+    <t>output_data/</t>
+  </si>
+  <si>
+    <t>output_figures/</t>
+  </si>
+  <si>
+    <t>Road_dust_parameter_table_example.xlsx</t>
+  </si>
+  <si>
+    <t>example_output.xlsx</t>
+  </si>
+  <si>
+    <t>output.txt</t>
   </si>
 </sst>
 </file>
@@ -562,7 +565,7 @@
         <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C2" t="s">
         <v>21</v>
@@ -579,7 +582,7 @@
         <v>0</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="4" spans="1:28" x14ac:dyDescent="0.2">
@@ -587,7 +590,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:28" x14ac:dyDescent="0.2">
@@ -595,7 +598,7 @@
         <v>7</v>
       </c>
       <c r="B5" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="6" spans="1:28" x14ac:dyDescent="0.2">
@@ -603,7 +606,7 @@
         <v>1</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>34</v>
       </c>
       <c r="C6" t="s">
         <v>20</v>
@@ -624,7 +627,7 @@
         <v>28</v>
       </c>
       <c r="AB6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="7" spans="1:28" x14ac:dyDescent="0.2">
@@ -641,6 +644,9 @@
       </c>
       <c r="B8" t="s">
         <v>35</v>
+      </c>
+      <c r="C8" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:28" x14ac:dyDescent="0.2">

</xml_diff>